<commit_message>
เพิ่ม mPayReport และแก้ Discout Report
</commit_message>
<xml_diff>
--- a/src/KE-PDC.Web/wwwroot/assets/templates/DailyRevenueConfirmReport.xlsx
+++ b/src/KE-PDC.Web/wwwroot/assets/templates/DailyRevenueConfirmReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkAtKerry\Program\WebApplication\PDC\PDCMaprole_Project\PDC\src\KE-PDC.Web\wwwroot\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ke-pdc-web-v2\ke-pdc-web-v2\src\KE-PDC.Web\wwwroot\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFF3EE2-E7C7-4D8A-8454-360AD4E95DBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE94E67-40EF-421E-93BD-ED636B44232E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9405" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4755" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Revenue Confirm" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>Freight</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Rabbit TopUp</t>
+  </si>
+  <si>
+    <t>MPay TopUp</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -876,12 +882,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1128,66 +1160,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="19" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="12" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="16" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="12" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="12" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1206,6 +1205,51 @@
     <xf numFmtId="166" fontId="5" fillId="11" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="19" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="19" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="19" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1227,22 +1271,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="19" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="19" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="19" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="19" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="HeaderStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1395,7 +1433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1691,13 +1729,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE5"/>
+  <dimension ref="A1:BG5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR18" sqref="AR18"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15"/>
@@ -1717,411 +1755,425 @@
     <col min="13" max="13" width="10.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="67" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="16.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="28" max="33" width="10.5703125" style="33" customWidth="1"/>
-    <col min="34" max="34" width="14.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.5703125" style="33" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16" style="32" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="32" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="16.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="30" max="35" width="10.5703125" style="33" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" style="33" customWidth="1"/>
+    <col min="38" max="38" width="13.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16" style="32" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.140625" style="34" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="13.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="14.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.42578125" style="34" customWidth="1"/>
-    <col min="47" max="47" width="14.7109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.5703125" style="73" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.7109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.7109375" style="38" customWidth="1"/>
-    <col min="54" max="54" width="15" style="39" customWidth="1"/>
-    <col min="55" max="55" width="7.140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.7109375" style="41" customWidth="1"/>
-    <col min="57" max="57" width="15" style="42" customWidth="1"/>
-    <col min="58" max="16384" width="8" style="43"/>
+    <col min="42" max="42" width="16.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="14.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" style="34" customWidth="1"/>
+    <col min="49" max="49" width="14.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.5703125" style="73" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.7109375" style="38" customWidth="1"/>
+    <col min="56" max="56" width="15" style="39" customWidth="1"/>
+    <col min="57" max="57" width="7.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.7109375" style="41" customWidth="1"/>
+    <col min="59" max="59" width="15" style="42" customWidth="1"/>
+    <col min="60" max="16384" width="8" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="57" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="104"/>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="108" t="s">
+    <row r="1" spans="1:59" s="57" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A1" s="91"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108"/>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="108"/>
-      <c r="AB1" s="108"/>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="108"/>
-      <c r="AF1" s="108"/>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="108"/>
-      <c r="AI1" s="108"/>
-      <c r="AJ1" s="108"/>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
-      <c r="AN1" s="108"/>
-      <c r="AO1" s="108"/>
-      <c r="AP1" s="108"/>
-      <c r="AQ1" s="108"/>
-      <c r="AR1" s="108"/>
-      <c r="AS1" s="108"/>
-      <c r="AT1" s="108"/>
-      <c r="AU1" s="108"/>
-      <c r="AV1" s="108"/>
-      <c r="AW1" s="108"/>
-      <c r="AX1" s="108"/>
-      <c r="AY1" s="108"/>
-      <c r="AZ1" s="108"/>
-      <c r="BA1" s="108"/>
-      <c r="BB1" s="108"/>
-      <c r="BC1" s="108"/>
-      <c r="BD1" s="108"/>
-      <c r="BE1" s="108"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="97"/>
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
+      <c r="AR1" s="97"/>
+      <c r="AS1" s="97"/>
+      <c r="AT1" s="97"/>
+      <c r="AU1" s="97"/>
+      <c r="AV1" s="97"/>
+      <c r="AW1" s="97"/>
+      <c r="AX1" s="97"/>
+      <c r="AY1" s="97"/>
+      <c r="AZ1" s="97"/>
+      <c r="BA1" s="97"/>
+      <c r="BB1" s="97"/>
+      <c r="BC1" s="97"/>
+      <c r="BD1" s="97"/>
+      <c r="BE1" s="97"/>
+      <c r="BF1" s="97"/>
+      <c r="BG1" s="97"/>
     </row>
-    <row r="2" spans="1:57" s="58" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="109" t="s">
+    <row r="2" spans="1:59" s="58" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
-      <c r="V2" s="109"/>
-      <c r="W2" s="109"/>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="109"/>
-      <c r="AC2" s="109"/>
-      <c r="AD2" s="109"/>
-      <c r="AE2" s="109"/>
-      <c r="AF2" s="109"/>
-      <c r="AG2" s="109"/>
-      <c r="AH2" s="109"/>
-      <c r="AI2" s="109"/>
-      <c r="AJ2" s="109"/>
-      <c r="AK2" s="109"/>
-      <c r="AL2" s="109"/>
-      <c r="AM2" s="109"/>
-      <c r="AN2" s="109"/>
-      <c r="AO2" s="109"/>
-      <c r="AP2" s="109"/>
-      <c r="AQ2" s="109"/>
-      <c r="AR2" s="109"/>
-      <c r="AS2" s="109"/>
-      <c r="AT2" s="109"/>
-      <c r="AU2" s="109"/>
-      <c r="AV2" s="109"/>
-      <c r="AW2" s="109"/>
-      <c r="AX2" s="109"/>
-      <c r="AY2" s="109"/>
-      <c r="AZ2" s="109"/>
-      <c r="BA2" s="109"/>
-      <c r="BB2" s="109"/>
-      <c r="BC2" s="109"/>
-      <c r="BD2" s="109"/>
-      <c r="BE2" s="109"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="98"/>
+      <c r="AI2" s="98"/>
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="98"/>
+      <c r="AM2" s="98"/>
+      <c r="AN2" s="98"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="98"/>
+      <c r="AQ2" s="98"/>
+      <c r="AR2" s="98"/>
+      <c r="AS2" s="98"/>
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="98"/>
+      <c r="AV2" s="98"/>
+      <c r="AW2" s="98"/>
+      <c r="AX2" s="98"/>
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="98"/>
+      <c r="BA2" s="98"/>
+      <c r="BB2" s="98"/>
+      <c r="BC2" s="98"/>
+      <c r="BD2" s="98"/>
+      <c r="BE2" s="98"/>
+      <c r="BF2" s="98"/>
+      <c r="BG2" s="98"/>
     </row>
-    <row r="3" spans="1:57" s="74" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A3" s="102" t="s">
+    <row r="3" spans="1:59" s="74" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="88" t="s">
+      <c r="J3" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="88" t="s">
+      <c r="K3" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="88" t="s">
+      <c r="L3" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="88" t="s">
+      <c r="N3" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="88" t="s">
+      <c r="O3" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="88" t="s">
+      <c r="P3" s="95" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="95" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="88" t="s">
+      <c r="S3" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="95" t="s">
+      <c r="T3" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="96"/>
-      <c r="T3" s="88" t="s">
+      <c r="U3" s="111"/>
+      <c r="V3" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="U3" s="88" t="s">
+      <c r="W3" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="88" t="s">
+      <c r="X3" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="88" t="s">
+      <c r="Y3" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="88" t="s">
+      <c r="Z3" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="88" t="s">
+      <c r="AA3" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="88" t="s">
+      <c r="AB3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="92" t="s">
+      <c r="AC3" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="92"/>
-      <c r="AD3" s="92"/>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="92"/>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="92"/>
-      <c r="AI3" s="92"/>
-      <c r="AJ3" s="88" t="s">
+      <c r="AD3" s="107"/>
+      <c r="AE3" s="107"/>
+      <c r="AF3" s="107"/>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="107"/>
+      <c r="AJ3" s="107"/>
+      <c r="AK3" s="107"/>
+      <c r="AL3" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="AK3" s="88" t="s">
+      <c r="AM3" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="AL3" s="121" t="s">
+      <c r="AN3" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="AM3" s="122"/>
-      <c r="AN3" s="122"/>
-      <c r="AO3" s="122"/>
-      <c r="AP3" s="122"/>
-      <c r="AQ3" s="122"/>
-      <c r="AR3" s="122"/>
-      <c r="AS3" s="122"/>
-      <c r="AT3" s="123"/>
-      <c r="AU3" s="97" t="s">
+      <c r="AO3" s="116"/>
+      <c r="AP3" s="116"/>
+      <c r="AQ3" s="116"/>
+      <c r="AR3" s="116"/>
+      <c r="AS3" s="116"/>
+      <c r="AT3" s="116"/>
+      <c r="AU3" s="116"/>
+      <c r="AV3" s="117"/>
+      <c r="AW3" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="AV3" s="98"/>
-      <c r="AW3" s="99"/>
-      <c r="AX3" s="93" t="s">
+      <c r="AX3" s="113"/>
+      <c r="AY3" s="114"/>
+      <c r="AZ3" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="AY3" s="106" t="s">
+      <c r="BA3" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="AZ3" s="90" t="s">
+      <c r="BB3" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="BA3" s="90"/>
-      <c r="BB3" s="90"/>
-      <c r="BC3" s="91" t="s">
+      <c r="BC3" s="105"/>
+      <c r="BD3" s="105"/>
+      <c r="BE3" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="BD3" s="91"/>
-      <c r="BE3" s="91"/>
+      <c r="BF3" s="106"/>
+      <c r="BG3" s="106"/>
     </row>
-    <row r="4" spans="1:57" s="87" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="103"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="75" t="s">
+    <row r="4" spans="1:59" s="87" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A4" s="90"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="76" t="s">
+      <c r="U4" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="89"/>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="77" t="s">
+      <c r="V4" s="96"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="96"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="96"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="78" t="s">
+      <c r="AD4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="AC4" s="78" t="s">
+      <c r="AE4" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="AD4" s="78" t="s">
+      <c r="AF4" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="AE4" s="78" t="s">
+      <c r="AG4" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="AF4" s="78" t="s">
+      <c r="AH4" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="AG4" s="78" t="s">
+      <c r="AI4" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="AH4" s="78" t="s">
+      <c r="AJ4" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="AI4" s="78" t="s">
+      <c r="AK4" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="79" t="s">
+      <c r="AL4" s="96"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="AM4" s="79" t="s">
+      <c r="AO4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="AN4" s="79" t="s">
+      <c r="AP4" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="AO4" s="79" t="s">
+      <c r="AQ4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="AP4" s="79" t="s">
+      <c r="AR4" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="AQ4" s="79" t="s">
+      <c r="AS4" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="79" t="s">
+      <c r="AT4" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="AS4" s="124" t="s">
+      <c r="AU4" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="AT4" s="124" t="s">
+      <c r="AV4" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="AU4" s="80" t="s">
+      <c r="AW4" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="AV4" s="80" t="s">
+      <c r="AX4" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="AW4" s="80" t="s">
+      <c r="AY4" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="AX4" s="94"/>
-      <c r="AY4" s="107"/>
-      <c r="AZ4" s="81" t="s">
+      <c r="AZ4" s="109"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="BA4" s="82" t="s">
+      <c r="BC4" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="BB4" s="83" t="s">
+      <c r="BD4" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="BC4" s="84" t="s">
+      <c r="BE4" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="BD4" s="85" t="s">
+      <c r="BF4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="BE4" s="86" t="s">
+      <c r="BG4" s="86" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:57" s="56" customFormat="1">
+    <row r="5" spans="1:59" s="56" customFormat="1">
       <c r="A5" s="70"/>
       <c r="B5" s="44"/>
       <c r="C5" s="68"/>
@@ -2139,28 +2191,28 @@
       <c r="O5" s="45"/>
       <c r="P5" s="45"/>
       <c r="Q5" s="45"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="47"/>
       <c r="V5" s="45"/>
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
       <c r="Y5" s="45"/>
       <c r="Z5" s="45"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="59"/>
       <c r="AD5" s="46"/>
       <c r="AE5" s="46"/>
       <c r="AF5" s="46"/>
       <c r="AG5" s="46"/>
       <c r="AH5" s="46"/>
       <c r="AI5" s="46"/>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="45"/>
-      <c r="AL5" s="47"/>
-      <c r="AM5" s="47"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="45"/>
+      <c r="AM5" s="45"/>
       <c r="AN5" s="47"/>
       <c r="AO5" s="47"/>
       <c r="AP5" s="47"/>
@@ -2168,64 +2220,68 @@
       <c r="AR5" s="47"/>
       <c r="AS5" s="47"/>
       <c r="AT5" s="47"/>
-      <c r="AU5" s="72"/>
-      <c r="AV5" s="72"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
       <c r="AW5" s="72"/>
-      <c r="AX5" s="48"/>
-      <c r="AY5" s="49"/>
-      <c r="AZ5" s="50"/>
-      <c r="BA5" s="51"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="53"/>
-      <c r="BD5" s="54"/>
-      <c r="BE5" s="55"/>
+      <c r="AX5" s="72"/>
+      <c r="AY5" s="72"/>
+      <c r="AZ5" s="48"/>
+      <c r="BA5" s="49"/>
+      <c r="BB5" s="50"/>
+      <c r="BC5" s="51"/>
+      <c r="BD5" s="52"/>
+      <c r="BE5" s="53"/>
+      <c r="BF5" s="54"/>
+      <c r="BG5" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="E1:BE1"/>
-    <mergeCell ref="E2:BE2"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="W3:W4"/>
+  <mergeCells count="39">
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="BB3:BD3"/>
+    <mergeCell ref="BE3:BG3"/>
+    <mergeCell ref="AC3:AK3"/>
+    <mergeCell ref="AZ3:AZ4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="AW3:AY3"/>
     <mergeCell ref="V3:V4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="AN3:AV3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="AA3:AI3"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="AU3:AW3"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="AL3:AT3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="BA3:BA4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="E1:BG1"/>
+    <mergeCell ref="E2:BG2"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="AZ5:AZ1048576">
+  <conditionalFormatting sqref="BB5:BB1048576">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BC5:BC1048576">
+  <conditionalFormatting sqref="BE5:BE1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -2269,104 +2325,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="114"/>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="118" t="s">
+      <c r="A1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="119"/>
-      <c r="AA1" s="119"/>
-      <c r="AB1" s="119"/>
-      <c r="AC1" s="119"/>
-      <c r="AD1" s="119"/>
-      <c r="AE1" s="119"/>
-      <c r="AF1" s="119"/>
-      <c r="AG1" s="119"/>
-      <c r="AH1" s="119"/>
-      <c r="AI1" s="119"/>
-      <c r="AJ1" s="119"/>
-      <c r="AK1" s="119"/>
-      <c r="AL1" s="119"/>
-      <c r="AM1" s="119"/>
-      <c r="AN1" s="119"/>
-      <c r="AO1" s="119"/>
-      <c r="AP1" s="119"/>
-      <c r="AQ1" s="119"/>
-      <c r="AR1" s="119"/>
-      <c r="AS1" s="119"/>
-      <c r="AT1" s="119"/>
-      <c r="AU1" s="120"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="123"/>
+      <c r="T1" s="123"/>
+      <c r="U1" s="123"/>
+      <c r="V1" s="123"/>
+      <c r="W1" s="123"/>
+      <c r="X1" s="123"/>
+      <c r="Y1" s="123"/>
+      <c r="Z1" s="123"/>
+      <c r="AA1" s="123"/>
+      <c r="AB1" s="123"/>
+      <c r="AC1" s="123"/>
+      <c r="AD1" s="123"/>
+      <c r="AE1" s="123"/>
+      <c r="AF1" s="123"/>
+      <c r="AG1" s="123"/>
+      <c r="AH1" s="123"/>
+      <c r="AI1" s="123"/>
+      <c r="AJ1" s="123"/>
+      <c r="AK1" s="123"/>
+      <c r="AL1" s="123"/>
+      <c r="AM1" s="123"/>
+      <c r="AN1" s="123"/>
+      <c r="AO1" s="123"/>
+      <c r="AP1" s="123"/>
+      <c r="AQ1" s="123"/>
+      <c r="AR1" s="123"/>
+      <c r="AS1" s="123"/>
+      <c r="AT1" s="123"/>
+      <c r="AU1" s="124"/>
     </row>
     <row r="2" spans="1:47" s="2" customFormat="1" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A2" s="116"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="119"/>
-      <c r="U2" s="119"/>
-      <c r="V2" s="119"/>
-      <c r="W2" s="119"/>
-      <c r="X2" s="119"/>
-      <c r="Y2" s="119"/>
-      <c r="Z2" s="119"/>
-      <c r="AA2" s="119"/>
-      <c r="AB2" s="119"/>
-      <c r="AC2" s="119"/>
-      <c r="AD2" s="119"/>
-      <c r="AE2" s="119"/>
-      <c r="AF2" s="119"/>
-      <c r="AG2" s="119"/>
-      <c r="AH2" s="119"/>
-      <c r="AI2" s="119"/>
-      <c r="AJ2" s="119"/>
-      <c r="AK2" s="119"/>
-      <c r="AL2" s="119"/>
-      <c r="AM2" s="119"/>
-      <c r="AN2" s="119"/>
-      <c r="AO2" s="119"/>
-      <c r="AP2" s="119"/>
-      <c r="AQ2" s="119"/>
-      <c r="AR2" s="119"/>
-      <c r="AS2" s="119"/>
-      <c r="AT2" s="119"/>
-      <c r="AU2" s="120"/>
+      <c r="A2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
+      <c r="AA2" s="123"/>
+      <c r="AB2" s="123"/>
+      <c r="AC2" s="123"/>
+      <c r="AD2" s="123"/>
+      <c r="AE2" s="123"/>
+      <c r="AF2" s="123"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="123"/>
+      <c r="AI2" s="123"/>
+      <c r="AJ2" s="123"/>
+      <c r="AK2" s="123"/>
+      <c r="AL2" s="123"/>
+      <c r="AM2" s="123"/>
+      <c r="AN2" s="123"/>
+      <c r="AO2" s="123"/>
+      <c r="AP2" s="123"/>
+      <c r="AQ2" s="123"/>
+      <c r="AR2" s="123"/>
+      <c r="AS2" s="123"/>
+      <c r="AT2" s="123"/>
+      <c r="AU2" s="124"/>
     </row>
     <row r="3" spans="1:47" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A3" s="22" t="s">

</xml_diff>